<commit_message>
Avance del flujo Emitir dictamen propuesta
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacion.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Cliente</t>
   </si>
@@ -86,12 +86,6 @@
     <t>MontoAmortizar</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>InteresRefinanciar</t>
-  </si>
-  <si>
     <t>Cronograma Pagos</t>
   </si>
   <si>
@@ -137,25 +131,28 @@
     <t>Pagare</t>
   </si>
   <si>
-    <t>080-01-8442351</t>
-  </si>
-  <si>
     <t>REFINANCIACION</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1069</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>prueba propuesta</t>
   </si>
   <si>
-    <t>16896616</t>
+    <t>1940821</t>
+  </si>
+  <si>
+    <t>080-01-9434661</t>
+  </si>
+  <si>
+    <t>808.46</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>42.58</t>
+  </si>
+  <si>
+    <t>4899906</t>
   </si>
 </sst>
 </file>
@@ -218,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -229,6 +226,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -523,21 +526,20 @@
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="30" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="33.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="30" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="33.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1">
+    <row r="1" spans="1:22" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -557,60 +559,57 @@
         <v>12</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>23</v>
+      <c r="M1" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="Q1" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="R1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="S1" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="T1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="U1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" s="4" customFormat="1">
+    <row r="2" spans="1:22" s="4" customFormat="1">
       <c r="A2" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>10</v>
@@ -619,89 +618,87 @@
         <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="J2" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="K2" s="6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>24</v>
+      <c r="M2" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="7" t="s">
+      <c r="P2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="V2"/>
-      <c r="W2"/>
     </row>
-    <row r="3" spans="1:23" s="4" customFormat="1">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-      <c r="P3"/>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
-      <c r="T3"/>
+    <row r="3" spans="1:22" s="4" customFormat="1">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
       <c r="U3"/>
       <c r="V3"/>
-      <c r="W3"/>
     </row>
-    <row r="7" spans="1:23">
-      <c r="O7" s="1"/>
+    <row r="7" spans="1:22">
+      <c r="N7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Registrar Aprobacion de propuestas credito empresrial
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacion.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Cliente</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Aprobado</t>
   </si>
   <si>
-    <t>Resultado</t>
-  </si>
-  <si>
     <t>Tipo Operación</t>
   </si>
   <si>
@@ -153,6 +150,15 @@
   </si>
   <si>
     <t>4899906</t>
+  </si>
+  <si>
+    <t>Resultado Emision Propuesta</t>
+  </si>
+  <si>
+    <t>Resultado Aprobador 1</t>
+  </si>
+  <si>
+    <t>okkkkkkkkkkkkkk</t>
   </si>
 </sst>
 </file>
@@ -215,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -232,6 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -537,9 +544,10 @@
     <col min="18" max="18" width="30" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="13.28515625" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="33.85546875" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1">
+    <row r="1" spans="1:23" s="4" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -559,10 +567,10 @@
         <v>12</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>19</v>
@@ -604,12 +612,15 @@
         <v>27</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="4" customFormat="1">
+    <row r="2" spans="1:23" s="4" customFormat="1">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>10</v>
@@ -618,7 +629,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>6</v>
@@ -627,13 +638,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>7</v>
@@ -648,16 +659,16 @@
         <v>23</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>8</v>
@@ -668,12 +679,15 @@
       <c r="T2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="U2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V2"/>
+      <c r="U2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2"/>
     </row>
-    <row r="3" spans="1:22" s="4" customFormat="1">
+    <row r="3" spans="1:23" s="4" customFormat="1">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -697,7 +711,7 @@
       <c r="U3"/>
       <c r="V3"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:23">
       <c r="N7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
proyecto integrado refinanciacion y reprogramacion 23122021
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacion.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacion.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CajaPiuraCMAC2021\target\DatosExcel\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Cliente</t>
   </si>
@@ -155,22 +155,20 @@
     <t>22296442</t>
   </si>
   <si>
-    <t>080-01-0178191</t>
-  </si>
-  <si>
-    <t>575.59</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>17006509</t>
+    <t>4899966</t>
+  </si>
+  <si>
+    <t>Se han encontrado errores en la Validacion de la Propuesta</t>
+  </si>
+  <si>
+    <t>El Documento ha sido derivado satisfactoriamente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -520,30 +518,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="30" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="33.85546875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="7" max="8" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="4" customFormat="1">
@@ -678,73 +674,39 @@
       <c r="T2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="U2"/>
-      <c r="V2"/>
+      <c r="U2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" t="s">
+        <v>44</v>
+      </c>
       <c r="W2"/>
     </row>
     <row r="3" spans="1:23" s="4" customFormat="1">
-      <c r="A3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="5" t="s">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3" t="s">
         <v>45</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="U3" s="7"/>
-      <c r="V3"/>
       <c r="W3"/>
     </row>
     <row r="7" spans="1:23">

</xml_diff>

<commit_message>
Proyecto Integrado para presentacion caja Piura
</commit_message>
<xml_diff>
--- a/target/DatosExcel/DatosCreditoEmpresarialRefinanciacion.xlsx
+++ b/target/DatosExcel/DatosCreditoEmpresarialRefinanciacion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Cliente</t>
   </si>
@@ -155,10 +155,25 @@
     <t>prueba</t>
   </si>
   <si>
-    <t>4899992</t>
-  </si>
-  <si>
-    <t>Se han encontrado errores en la Validacion de la Propuesta</t>
+    <t>7993234</t>
+  </si>
+  <si>
+    <t>080-01-9179211</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>4900005</t>
+  </si>
+  <si>
+    <t>4900006</t>
+  </si>
+  <si>
+    <t>4900007</t>
+  </si>
+  <si>
+    <t>El Documento ha sido derivado satisfactoriamente</t>
   </si>
 </sst>
 </file>
@@ -207,11 +222,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,15 +508,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="54.0" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="54.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -574,75 +590,144 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="U2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>43</v>
       </c>
-      <c r="V2" t="s">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
         <v>44</v>
+      </c>
+      <c r="I3">
+        <v>896.22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>